<commit_message>
do dl buoi hoc
</commit_message>
<xml_diff>
--- a/database/seeders/_buoi_hoc_seeder.xlsx
+++ b/database/seeders/_buoi_hoc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="buoi_hoc" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Đã kết thúc</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>buoi_hoc_id</t>
+  </si>
+  <si>
+    <t>hoc_sinh_id</t>
+  </si>
+  <si>
+    <t>ketqua</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -574,13 +580,208 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix nut buoi hoc
</commit_message>
<xml_diff>
--- a/database/seeders/_buoi_hoc_seeder.xlsx
+++ b/database/seeders/_buoi_hoc_seeder.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\DoAn\database\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\source\repos\DoAn_Final\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB5C45C-775F-4A4B-A50A-6319C227253E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="buoi_hoc" sheetId="2" r:id="rId1"/>
@@ -87,12 +86,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -399,25 +398,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="17.25" customWidth="1"/>
-    <col min="6" max="6" width="12.625" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -443,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -466,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -489,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -558,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
@@ -567,12 +566,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -580,20 +579,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -604,7 +603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -615,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -626,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -637,7 +636,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -648,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -659,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -670,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -681,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -692,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -703,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -714,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -725,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -736,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -747,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -758,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -769,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -787,44 +786,44 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>